<commit_message>
add localization to text set at runtime
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="102">
   <si>
     <t>Key</t>
   </si>
@@ -308,6 +308,18 @@
   </si>
   <si>
     <t>GAME_NAME</t>
+  </si>
+  <si>
+    <t>UI_GAME_TARGET</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>FORMATTED_UI_GAME_TARGET</t>
+  </si>
+  <si>
+    <t>Target: {0}</t>
   </si>
 </sst>
 </file>
@@ -375,7 +387,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -690,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1456,10 +1482,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>5</v>
@@ -1473,10 +1499,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>5</v>
@@ -1490,24 +1516,58 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="4" t="s">
+      <c r="C48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Reorganise models into folders Add wave images to be used instead of particle effect Set linux build to start as server automatically set webgl build to read config for address and port to connect to and join automatically Add ShowMenu flag to MainMenu for testing purposes
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="104">
   <si>
     <t>Key</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t>Target: {0}</t>
+  </si>
+  <si>
+    <t>BUTTON_CANCEL</t>
+  </si>
+  <si>
+    <t>Cancel</t>
   </si>
 </sst>
 </file>
@@ -695,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -951,10 +957,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>5</v>
@@ -968,10 +974,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>5</v>
@@ -985,10 +991,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>5</v>
@@ -1002,10 +1008,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>5</v>
@@ -1019,10 +1025,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>5</v>
@@ -1036,10 +1042,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>5</v>
@@ -1053,10 +1059,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>5</v>
@@ -1070,10 +1076,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>5</v>
@@ -1087,10 +1093,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>5</v>
@@ -1104,10 +1110,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>5</v>
@@ -1121,10 +1127,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>5</v>
@@ -1138,10 +1144,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>5</v>
@@ -1155,10 +1161,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>5</v>
@@ -1172,10 +1178,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>5</v>
@@ -1189,10 +1195,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>5</v>
@@ -1206,10 +1212,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>5</v>
@@ -1223,10 +1229,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>5</v>
@@ -1240,44 +1246,44 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="C33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>5</v>
@@ -1291,27 +1297,27 @@
     </row>
     <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>5</v>
@@ -1325,10 +1331,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>5</v>
@@ -1342,10 +1348,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>5</v>
@@ -1359,10 +1365,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>5</v>
@@ -1376,10 +1382,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>5</v>
@@ -1393,10 +1399,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>5</v>
@@ -1410,10 +1416,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>5</v>
@@ -1427,10 +1433,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>5</v>
@@ -1444,10 +1450,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>5</v>
@@ -1461,10 +1467,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>5</v>
@@ -1478,10 +1484,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>5</v>
@@ -1495,10 +1501,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>5</v>
@@ -1512,10 +1518,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>5</v>
@@ -1529,18 +1535,35 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="4" t="s">
+      <c r="C50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add waiting for other players message whilst other players are selecting their characters
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="106">
   <si>
     <t>Key</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t>Cancel</t>
+  </si>
+  <si>
+    <t>UI_GAME_WAITING_FOR_PLAYERS</t>
+  </si>
+  <si>
+    <t>Waiting for other players…</t>
   </si>
 </sst>
 </file>
@@ -701,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1501,10 +1507,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>5</v>
@@ -1518,10 +1524,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>5</v>
@@ -1535,10 +1541,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>5</v>
@@ -1552,18 +1558,35 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="4" t="s">
+      <c r="C51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
move target to above chest and current total to the bridge so that it can be seen at all times
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="108">
   <si>
     <t>Key</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>Waiting for other players…</t>
+  </si>
+  <si>
+    <t>FORMATTED_UI_GAME_CURRENT</t>
+  </si>
+  <si>
+    <t>Current Total: {0}</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -707,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1590,9 +1603,26 @@
         <v>5</v>
       </c>
     </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add space bar and arrow key icons
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/LocalizationStrings.xlsx
@@ -405,14 +405,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -722,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1622,7 +1615,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"XXXX"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
drop how to play screen remove how to play text
</commit_message>
<xml_diff>
--- a/Assets/Localization/Editor/LocalizationStrings.xlsx
+++ b/Assets/Localization/Editor/LocalizationStrings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="90">
   <si>
     <t>Key</t>
   </si>
@@ -166,57 +166,6 @@
     <t>UI_END_ROUNDS_COMPLETED</t>
   </si>
   <si>
-    <t>UI_INSTRUCTIONS_TITLE</t>
-  </si>
-  <si>
-    <t>UI_INSTRUCTIONS_AIM</t>
-  </si>
-  <si>
-    <t>UI_INSTRUCTIONS_CONTROLS</t>
-  </si>
-  <si>
-    <t>UI_INSTRUCTIONS_ROLES</t>
-  </si>
-  <si>
-    <t>UI_INSTRUCTIONS_PUSHER</t>
-  </si>
-  <si>
-    <t>UI_INSTRUCTIONS_SURFER</t>
-  </si>
-  <si>
-    <t>UI_INSTRUCTIONS_AIM_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>UI_INSTRUCTIONS_SURFER_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>UI_INSTRUCTIONS_PUSHER_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>How to Play</t>
-  </si>
-  <si>
-    <t>Aim of the Game</t>
-  </si>
-  <si>
-    <t>WASD - Move, SPACE - Interact</t>
-  </si>
-  <si>
-    <t>Roles</t>
-  </si>
-  <si>
-    <t>Pusher</t>
-  </si>
-  <si>
-    <t>Surfer</t>
-  </si>
-  <si>
-    <t>Use your oar to push the player.\n\nIt is your responsibility to make sure that the surfer makes it to the chest</t>
-  </si>
-  <si>
-    <t>You must surf on the platform to get to the chest with the help of the pushers.\n\nYou must then distribute rewards amongst your crew</t>
-  </si>
-  <si>
     <t>UI_CHARACTER_TITLE</t>
   </si>
   <si>
@@ -263,9 +212,6 @@
   </si>
   <si>
     <t>Work together to get from the bridge to the chest</t>
-  </si>
-  <si>
-    <t>Work together to get from the bridge to the chest to claim your reward.\n\nThe chest can only be opened when you have reached the target value using the operations available</t>
   </si>
   <si>
     <t>FORMATTED_UI_END_ROUNDS_COMPLETED</t>
@@ -713,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -748,7 +694,7 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>25</v>
@@ -918,10 +864,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>5</v>
@@ -935,10 +881,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>5</v>
@@ -952,10 +898,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>5</v>
@@ -969,10 +915,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>5</v>
@@ -989,7 +935,7 @@
         <v>45</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>5</v>
@@ -1193,7 +1139,7 @@
         <v>50</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>5</v>
@@ -1207,10 +1153,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>5</v>
@@ -1224,10 +1170,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>5</v>
@@ -1241,7 +1187,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>62</v>
@@ -1258,10 +1204,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>5</v>
@@ -1275,10 +1221,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>5</v>
@@ -1290,12 +1236,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>5</v>
@@ -1307,12 +1253,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>5</v>
@@ -1324,12 +1270,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>5</v>
@@ -1343,10 +1289,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>5</v>
@@ -1360,10 +1306,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>5</v>
@@ -1377,10 +1323,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>5</v>
@@ -1394,10 +1340,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>5</v>
@@ -1411,10 +1357,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>5</v>
@@ -1428,10 +1374,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>5</v>
@@ -1445,10 +1391,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>5</v>
@@ -1457,159 +1403,6 @@
         <v>5</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>